<commit_message>
i hate it here
</commit_message>
<xml_diff>
--- a/P06/Scrum_Sprint_2.xlsx
+++ b/P06/Scrum_Sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachaelrocha/Documents/GitHub/cse1325/P06/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3D1568-8398-444E-9058-CA39E5D2FE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF04D65-971A-3A42-86B3-5D63F4FEDA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16980" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="171">
   <si>
     <t>Product Name:</t>
   </si>
@@ -552,6 +552,9 @@
   </si>
   <si>
     <t>Inserted Computer Information</t>
+  </si>
+  <si>
+    <t>List  data on display</t>
   </si>
 </sst>
 </file>
@@ -1679,22 +1682,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -6867,8 +6870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6973,7 +6976,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -6988,7 +6991,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -7006,7 +7009,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -7024,7 +7027,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -7042,7 +7045,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -7060,7 +7063,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -7082,7 +7085,7 @@
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
@@ -7286,14 +7289,20 @@
       <c r="E26" s="37"/>
       <c r="F26" s="38"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4">
         <v>11</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="35" t="s">
+        <v>61</v>
+      </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="37"/>
+      <c r="D27" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>167</v>
+      </c>
       <c r="F27" s="38"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>